<commit_message>
Updated the sheet so it can quickly add more permissions to the existing identities
</commit_message>
<xml_diff>
--- a/SmallSimilarityExample.xlsx
+++ b/SmallSimilarityExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jreshef\Documents\Projects\PermissionAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F436C17C-3675-4064-83AF-B4FB08977D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B50C91-EF3A-479A-9026-54CEF95B742E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={87B74879-7227-48D1-8D39-65E466AE20C9}</author>
+    <author>tc={46A0C6C7-CEEF-471F-AA3C-125D5D8932D2}</author>
+    <author>tc={2B65ED7F-3712-4AC2-80D1-0E4D2BC0C51C}</author>
+  </authors>
+  <commentList>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{87B74879-7227-48D1-8D39-65E466AE20C9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dot product with other identities</t>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="1" shapeId="0" xr:uid="{46A0C6C7-CEEF-471F-AA3C-125D5D8932D2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Dot product with self to normalise</t>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="2" shapeId="0" xr:uid="{2B65ED7F-3712-4AC2-80D1-0E4D2BC0C51C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Normalised dot product</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -53,12 +89,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
   <si>
     <t>Raw data</t>
-  </si>
-  <si>
-    <t>Similarity</t>
   </si>
   <si>
     <t>A</t>
@@ -72,12 +105,18 @@
   <si>
     <t>D</t>
   </si>
+  <si>
+    <t>Similarity score</t>
+  </si>
+  <si>
+    <t>Calculations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +128,18 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -119,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -151,6 +202,15 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -166,6 +226,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jonathan Reshef (NZ)" id="{A63E3B2E-5D49-4514-B5CA-9BB59FEBD115}" userId="S::jono.x.reshef@pwc.com::47783a57-b5dd-4a8b-88d7-022e33e20372" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,24 +517,38 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G3" dT="2022-11-23T03:01:22.23" personId="{A63E3B2E-5D49-4514-B5CA-9BB59FEBD115}" id="{87B74879-7227-48D1-8D39-65E466AE20C9}">
+    <text>Dot product with other identities</text>
+  </threadedComment>
+  <threadedComment ref="G7" dT="2022-11-23T03:01:37.99" personId="{A63E3B2E-5D49-4514-B5CA-9BB59FEBD115}" id="{46A0C6C7-CEEF-471F-AA3C-125D5D8932D2}">
+    <text>Dot product with self to normalise</text>
+  </threadedComment>
+  <threadedComment ref="G11" dT="2022-11-23T03:02:15.93" personId="{A63E3B2E-5D49-4514-B5CA-9BB59FEBD115}" id="{2B65ED7F-3712-4AC2-80D1-0E4D2BC0C51C}">
+    <text>Normalised dot product</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="8.5546875" style="8"/>
     <col min="5" max="5" width="8.5546875" style="9"/>
-    <col min="6" max="6" width="0" style="9" hidden="1" customWidth="1"/>
-    <col min="7" max="9" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0" style="11" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="9" hidden="1" customWidth="1"/>
+    <col min="7" max="9" width="8.5546875" style="10" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" style="11" hidden="1" customWidth="1"/>
     <col min="11" max="12" width="8.5546875" style="9"/>
     <col min="13" max="16" width="8.5546875" style="12"/>
   </cols>
@@ -482,14 +562,16 @@
       <c r="D1" s="13"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
+      <c r="G1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N1" s="14"/>
       <c r="O1" s="14"/>
@@ -497,44 +579,44 @@
     </row>
     <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -542,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6">
         <v>0</v>
@@ -552,40 +634,40 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="6">
-        <f>SUMPRODUCT($A$3:$A$10,A$3:A$10)</f>
+        <f>SUMPRODUCT($A$3:$A$100,A$3:A$100)</f>
+        <v>10</v>
+      </c>
+      <c r="H3" s="6">
+        <f>SUMPRODUCT($A$3:$A$100,B$3:B$100)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="6">
+        <f>SUMPRODUCT($A$3:$A$100,C$3:C$100)</f>
+        <v>7</v>
+      </c>
+      <c r="J3" s="6">
+        <f>SUMPRODUCT($A$3:$A$100,D$3:D$100)</f>
         <v>5</v>
-      </c>
-      <c r="H3" s="6">
-        <f>SUMPRODUCT($A$3:$A$10,B$3:B$10)</f>
-        <v>4</v>
-      </c>
-      <c r="I3" s="6">
-        <f>SUMPRODUCT($A$3:$A$10,C$3:C$10)</f>
-        <v>4</v>
-      </c>
-      <c r="J3" s="6">
-        <f>SUMPRODUCT($A$3:$A$10,D$3:D$10)</f>
-        <v>3</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3" s="7" cm="1">
         <f t="array" ref="M3:P6">G11:J14*TRANSPOSE(G11:J14)</f>
         <v>1</v>
       </c>
       <c r="N3" s="7">
-        <v>0.64000000000000012</v>
+        <v>0.2</v>
       </c>
       <c r="O3" s="7">
-        <v>0.64000000000000012</v>
+        <v>0.7</v>
       </c>
       <c r="P3" s="7">
-        <v>0.44999999999999996</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -593,7 +675,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -603,44 +685,44 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" s="6">
-        <f>SUMPRODUCT($B$3:$B$10,A$3:A$10)</f>
-        <v>4</v>
+        <f>SUMPRODUCT($B$3:$B$100,A$3:A$100)</f>
+        <v>2</v>
       </c>
       <c r="H4" s="6">
-        <f>SUMPRODUCT($B$3:$B$10,B$3:B$10)</f>
-        <v>5</v>
+        <f>SUMPRODUCT($B$3:$B$100,B$3:B$100)</f>
+        <v>2</v>
       </c>
       <c r="I4" s="6">
-        <f>SUMPRODUCT($B$3:$B$10,C$3:C$10)</f>
-        <v>4</v>
+        <f>SUMPRODUCT($B$3:$B$100,C$3:C$100)</f>
+        <v>0</v>
       </c>
       <c r="J4" s="6">
-        <f>SUMPRODUCT($B$3:$B$10,D$3:D$10)</f>
-        <v>3</v>
+        <f>SUMPRODUCT($B$3:$B$100,D$3:D$100)</f>
+        <v>2</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="7">
-        <v>0.64000000000000012</v>
+        <v>2</v>
+      </c>
+      <c r="M4" s="16">
+        <v>0.2</v>
       </c>
       <c r="N4" s="7">
         <v>1</v>
       </c>
       <c r="O4" s="7">
-        <v>0.64000000000000012</v>
+        <v>0</v>
       </c>
       <c r="P4" s="7">
-        <v>0.44999999999999996</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
@@ -653,44 +735,44 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="6">
-        <f>SUMPRODUCT($C$3:$C$10,A$3:A$10)</f>
-        <v>4</v>
+        <f>SUMPRODUCT($C$3:$C$100,A$3:A$100)</f>
+        <v>7</v>
       </c>
       <c r="H5" s="6">
-        <f>SUMPRODUCT($C$3:$C$10,B$3:B$10)</f>
-        <v>4</v>
+        <f>SUMPRODUCT($C$3:$C$100,B$3:B$100)</f>
+        <v>0</v>
       </c>
       <c r="I5" s="6">
-        <f>SUMPRODUCT($C$3:$C$10,C$3:C$10)</f>
-        <v>5</v>
+        <f>SUMPRODUCT($C$3:$C$100,C$3:C$100)</f>
+        <v>7</v>
       </c>
       <c r="J5" s="6">
-        <f>SUMPRODUCT($C$3:$C$10,D$3:D$10)</f>
-        <v>2</v>
+        <f>SUMPRODUCT($C$3:$C$100,D$3:D$100)</f>
+        <v>3</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M5" s="7">
-        <v>0.64000000000000012</v>
-      </c>
-      <c r="N5" s="7">
-        <v>0.64000000000000012</v>
+        <v>3</v>
+      </c>
+      <c r="M5" s="16">
+        <v>0.7</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0</v>
       </c>
       <c r="O5" s="7">
         <v>1</v>
       </c>
       <c r="P5" s="7">
-        <v>0.2</v>
+        <v>0.25714285714285712</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="6">
         <v>0</v>
@@ -703,38 +785,38 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6">
+        <f>SUMPRODUCT($D$3:$D$100,A$3:A$100)</f>
         <v>5</v>
       </c>
-      <c r="G6" s="6">
-        <f>SUMPRODUCT($D$3:$D$10,A$3:A$10)</f>
+      <c r="H6" s="6">
+        <f>SUMPRODUCT($D$3:$D$100,B$3:B$100)</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="6">
+        <f>SUMPRODUCT($D$3:$D$100,C$3:C$100)</f>
         <v>3</v>
       </c>
-      <c r="H6" s="6">
-        <f>SUMPRODUCT($D$3:$D$10,B$3:B$10)</f>
-        <v>3</v>
-      </c>
-      <c r="I6" s="6">
-        <f>SUMPRODUCT($D$3:$D$10,C$3:C$10)</f>
-        <v>2</v>
-      </c>
       <c r="J6" s="6">
-        <f>SUMPRODUCT($D$3:$D$10,D$3:D$10)</f>
-        <v>4</v>
+        <f>SUMPRODUCT($D$3:$D$100,D$3:D$100)</f>
+        <v>5</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="M6" s="7">
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="N6" s="7">
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="O6" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="P6" s="7">
+        <v>4</v>
+      </c>
+      <c r="M6" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0.25714285714285712</v>
+      </c>
+      <c r="P6" s="15">
         <v>1</v>
       </c>
     </row>
@@ -743,33 +825,33 @@
         <v>1</v>
       </c>
       <c r="B7" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
       </c>
       <c r="D7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="6">
-        <f t="shared" ref="G7:J10" si="0">SUMPRODUCT(A$3:A$10)</f>
+        <f>SUMPRODUCT(A$3:A$100)</f>
+        <v>10</v>
+      </c>
+      <c r="H7" s="6">
+        <f>SUMPRODUCT(B$3:B$100)</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="6">
+        <f>SUMPRODUCT(C$3:C$100)</f>
+        <v>7</v>
+      </c>
+      <c r="J7" s="6">
+        <f>SUMPRODUCT(D$3:D$100)</f>
         <v>5</v>
-      </c>
-      <c r="H7" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J7" s="6">
-        <f t="shared" si="0"/>
-        <v>4</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -783,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -793,23 +875,23 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="6">
-        <f t="shared" si="0"/>
+        <f>SUMPRODUCT(A$3:A$100)</f>
+        <v>10</v>
+      </c>
+      <c r="H8" s="6">
+        <f>SUMPRODUCT(B$3:B$100)</f>
+        <v>2</v>
+      </c>
+      <c r="I8" s="6">
+        <f>SUMPRODUCT(C$3:C$100)</f>
+        <v>7</v>
+      </c>
+      <c r="J8" s="6">
+        <f>SUMPRODUCT(D$3:D$100)</f>
         <v>5</v>
-      </c>
-      <c r="H8" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J8" s="6">
-        <f t="shared" si="0"/>
-        <v>4</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -820,7 +902,7 @@
     </row>
     <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="6">
         <v>0</v>
@@ -833,23 +915,23 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="6">
-        <f t="shared" si="0"/>
+        <f>SUMPRODUCT(A$3:A$100)</f>
+        <v>10</v>
+      </c>
+      <c r="H9" s="6">
+        <f>SUMPRODUCT(B$3:B$100)</f>
+        <v>2</v>
+      </c>
+      <c r="I9" s="6">
+        <f>SUMPRODUCT(C$3:C$100)</f>
+        <v>7</v>
+      </c>
+      <c r="J9" s="6">
+        <f>SUMPRODUCT(D$3:D$100)</f>
         <v>5</v>
-      </c>
-      <c r="H9" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I9" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J9" s="6">
-        <f t="shared" si="0"/>
-        <v>4</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -863,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -873,23 +955,23 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="6">
+        <f>SUMPRODUCT(A$3:A$100)</f>
+        <v>10</v>
+      </c>
+      <c r="H10" s="6">
+        <f>SUMPRODUCT(B$3:B$100)</f>
+        <v>2</v>
+      </c>
+      <c r="I10" s="6">
+        <f>SUMPRODUCT(C$3:C$100)</f>
+        <v>7</v>
+      </c>
+      <c r="J10" s="6">
+        <f>SUMPRODUCT(D$3:D$100)</f>
         <v>5</v>
-      </c>
-      <c r="G10" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H10" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I10" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J10" s="6">
-        <f t="shared" si="0"/>
-        <v>4</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -899,27 +981,35 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="6">
-        <f t="shared" ref="G11:J14" si="1">G3/G7</f>
+        <f t="shared" ref="G11:J14" si="0">G3/G7</f>
         <v>1</v>
       </c>
       <c r="H11" s="7">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -929,27 +1019,35 @@
       <c r="P11" s="5"/>
     </row>
     <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="6">
+        <v>1</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="7">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I12" s="7">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f t="shared" si="0"/>
+        <v>0.4</v>
       </c>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -966,20 +1064,20 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="7">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
       <c r="H13" s="7">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -996,19 +1094,19 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="H14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I14" s="7">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
+        <f t="shared" si="0"/>
+        <v>0.42857142857142855</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K14" s="1"/>
@@ -1019,11 +1117,12 @@
       <c r="P14" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="M1:P1"/>
+    <mergeCell ref="G1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:D10">
+  <conditionalFormatting sqref="A3:D12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1035,7 +1134,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M3:P6">
+  <conditionalFormatting sqref="M3:P3 P6 O5:P5 N4:P4">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1048,5 +1147,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>